<commit_message>
Update de la liste des optimisations et du modèle audit SEO (Changement de l'optimisation 4 et ajout de 2 autres / correction typographique et ajout d'une entrée dans le modèle audit)
</commit_message>
<xml_diff>
--- a/rapport/Modèle-audit-SEO.xlsx
+++ b/rapport/Modèle-audit-SEO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
   <si>
     <t>Catégorie</t>
   </si>
@@ -109,6 +109,9 @@
     <t>https://fr.semrush.com/blog/seo-black-hat/   //    https://moz.com/learn/seo/anchor-text    //   https://www.abondance.com/20170117-17472-crawl-budget-google-explique-vision.html</t>
   </si>
   <si>
+    <t>SEO/Accessibilité</t>
+  </si>
+  <si>
     <t>Images contenant du texte</t>
   </si>
   <si>
@@ -124,7 +127,7 @@
     <t>https://dopweb.com/heading-tags-seo/</t>
   </si>
   <si>
-    <t>Images au format bpm</t>
+    <t>Images au format bmp</t>
   </si>
   <si>
     <t>Egalement cela rend le contenu trop lourd</t>
@@ -139,9 +142,6 @@
     <t>https://imageseo.io/images-seo-optimization/#:~:text=Image%20Format%20SEO%20Recommendations%3B%20JPG%20%2F%20JPEG%3A%20Prioritize,download%20SVG%20from%20websites%20you%20don%E2%80%99t%20trust.%20WebP</t>
   </si>
   <si>
-    <t>SEO/Accessibilité</t>
-  </si>
-  <si>
     <t>Absence de valeurs sémantiques</t>
   </si>
   <si>
@@ -260,6 +260,21 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Contenu de la balise meta keywords incorrect</t>
+  </si>
+  <si>
+    <t>Le contenu de la balise meta keywords manque de pertinence et comporte des répétitions.</t>
+  </si>
+  <si>
+    <t>Lister et cibler en amont de la création un nombre de mot décrivant précisément le site</t>
+  </si>
+  <si>
+    <t>Modifier le contenu de la balise et supprimer les répétitions</t>
+  </si>
+  <si>
+    <t>https://www.semrush.com/blog/meta-keywords/?kw=&amp;cmp=FR_SRCH_DSA_Blog_Core_BU_EN&amp;label=dsa_pagefeed&amp;Network=g&amp;Device=c&amp;utm_content=484898613071&amp;kwid=dsa-1053501803507&amp;cmpid=11794203801&amp;agpid=114205323586&amp;BU=Core&amp;extid=205227547929&amp;adpos=&amp;gclid=CjwKCAiA1uKMBhAGEiwAxzvX9-tJ5az7VWjSO0IdCkmukIUY2X2kvBLsxYlHiHs86F943AKWSrASQhoCGDcQAvD_BwE</t>
   </si>
 </sst>
 </file>
@@ -301,11 +316,7 @@
       <u/>
       <color rgb="FF0563C1"/>
     </font>
-    <font>
-      <u/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-    </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -341,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -372,7 +383,10 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
@@ -599,7 +613,7 @@
     <col customWidth="1" min="1" max="1" width="23.11"/>
     <col customWidth="1" min="2" max="2" width="40.78"/>
     <col customWidth="1" min="3" max="3" width="103.67"/>
-    <col customWidth="1" min="4" max="4" width="62.89"/>
+    <col customWidth="1" min="4" max="4" width="64.89"/>
     <col customWidth="1" min="5" max="5" width="46.44"/>
     <col customWidth="1" min="6" max="6" width="126.89"/>
     <col customWidth="1" min="7" max="26" width="10.56"/>
@@ -757,7 +771,7 @@
       <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -766,23 +780,23 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>6</v>
+      <c r="A12" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -793,20 +807,20 @@
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
+      <c r="B14" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="12" t="s">
         <v>41</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -814,7 +828,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>43</v>
@@ -828,7 +842,7 @@
       <c r="E16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="14" t="s">
         <v>47</v>
       </c>
     </row>
@@ -837,7 +851,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>48</v>
@@ -851,7 +865,7 @@
       <c r="E18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -860,7 +874,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>53</v>
@@ -874,7 +888,7 @@
       <c r="E20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>57</v>
       </c>
     </row>
@@ -920,7 +934,7 @@
       <c r="E24" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -943,7 +957,7 @@
       <c r="E26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="13" t="s">
         <v>72</v>
       </c>
     </row>
@@ -952,7 +966,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>73</v>
@@ -1002,8 +1016,24 @@
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="7"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="7"/>
@@ -3925,10 +3955,11 @@
     <hyperlink r:id="rId12" ref="F26"/>
     <hyperlink r:id="rId13" ref="F28"/>
     <hyperlink r:id="rId14" ref="F30"/>
+    <hyperlink r:id="rId15" ref="F32"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>